<commit_message>
Score Multiplier Messages: Content - Removed nested nodes so it works with the new DefinitionNode XML parser.
Former-commit-id: 9e3c2d86f2812f578920414fed00feb7c082ff45
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Multipliers.xlsx
+++ b/Docs/Content/HungryDragonContent_Multipliers.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7B67D3-E596-45E8-9437-05C5B62C6FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35640" yWindow="645" windowWidth="37395" windowHeight="21135"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="score" sheetId="4" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -107,9 +108,6 @@
     <t>SURVIVAL BONUS DEFINITIONS</t>
   </si>
   <si>
-    <t>&lt;FeedbackMessage&gt;</t>
-  </si>
-  <si>
     <t>multiplier_8</t>
   </si>
   <si>
@@ -155,42 +153,6 @@
     <t>SCORE MULTIPLIER DEFINITIONS</t>
   </si>
   <si>
-    <t>TID_FEEDBACK_SCORE_X1_01</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X1_02</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X1_03</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X2_01</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X2_02</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X2_03</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X3_01</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X3_02</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X3_03</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X4_01</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X4_02</t>
-  </si>
-  <si>
-    <t>TID_FEEDBACK_SCORE_X4_03</t>
-  </si>
-  <si>
     <t>TID_FEEDBACK_SCORE_X5_01</t>
   </si>
   <si>
@@ -201,12 +163,24 @@
   </si>
   <si>
     <t>TID_FEEDBACK_SCORE_X8_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X1_01;TID_FEEDBACK_SCORE_X1_02;TID_FEEDBACK_SCORE_X1_03</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X2_01;TID_FEEDBACK_SCORE_X2_02;TID_FEEDBACK_SCORE_X2_03</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X3_01;TID_FEEDBACK_SCORE_X3_02;TID_FEEDBACK_SCORE_X3_03</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X4_01;TID_FEEDBACK_SCORE_X4_02;TID_FEEDBACK_SCORE_X4_03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,18 +266,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -314,14 +276,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -399,19 +355,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -434,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -444,24 +387,23 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -481,12 +423,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -610,30 +546,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -867,13 +803,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -884,6 +813,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -943,29 +879,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="scoreMultiplierDefinitions2" displayName="scoreMultiplierDefinitions2" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
-  <autoFilter ref="B4:H29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="scoreMultiplierDefinitions2" displayName="scoreMultiplierDefinitions2" ref="B4:H13" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="B4:H13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="scoreMultiplierDefinitions19283" displayName="scoreMultiplierDefinitions19283" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="B35:E45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="scoreMultiplierDefinitions19283" displayName="scoreMultiplierDefinitions19283" ref="B19:E29" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B19:E29" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1233,14 +1169,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:K50"/>
+  <dimension ref="B1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,14 +1187,14 @@
     <col min="4" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="8" max="8" width="119" customWidth="1"/>
     <col min="9" max="28" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1271,658 +1207,466 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="30"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:11" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="27">
-        <v>0</v>
-      </c>
-      <c r="E5" s="26">
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21">
         <v>1</v>
       </c>
-      <c r="F5" s="26">
-        <v>0</v>
-      </c>
-      <c r="G5" s="26">
+      <c r="F5" s="21">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21">
         <v>-1</v>
       </c>
-      <c r="H5" s="25"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="24">
         <v>2</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="24">
         <v>8</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="24">
         <v>3</v>
       </c>
-      <c r="H6" s="25"/>
+      <c r="H6" s="20" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="22">
+        <v>2</v>
+      </c>
+      <c r="E7" s="21">
+        <v>4</v>
+      </c>
+      <c r="F7" s="21">
+        <v>22</v>
+      </c>
+      <c r="G7" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="22">
+        <v>3</v>
+      </c>
+      <c r="E8" s="21">
+        <v>6</v>
+      </c>
+      <c r="F8" s="21">
+        <v>32</v>
+      </c>
+      <c r="G8" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="22">
+        <v>4</v>
+      </c>
+      <c r="E9" s="21">
+        <v>8</v>
+      </c>
+      <c r="F9" s="21">
+        <v>50</v>
+      </c>
+      <c r="G9" s="21">
+        <v>2</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="22">
+        <v>5</v>
+      </c>
+      <c r="E10" s="21">
+        <v>10</v>
+      </c>
+      <c r="F10" s="21">
+        <v>75</v>
+      </c>
+      <c r="G10" s="21">
+        <v>2</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="22">
+        <v>6</v>
+      </c>
+      <c r="E11" s="21">
+        <v>12</v>
+      </c>
+      <c r="F11" s="21">
+        <v>120</v>
+      </c>
+      <c r="G11" s="21">
+        <v>2</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="22">
+        <v>7</v>
+      </c>
+      <c r="E12" s="21">
+        <v>14</v>
+      </c>
+      <c r="F12" s="21">
+        <v>5000</v>
+      </c>
+      <c r="G12" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="21" t="s">
+      <c r="D13" s="22">
+        <v>8</v>
+      </c>
+      <c r="E13" s="21">
+        <v>16</v>
+      </c>
+      <c r="F13" s="21">
+        <v>5000</v>
+      </c>
+      <c r="G13" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="27">
+    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="19" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="26">
+      <c r="D19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="16">
+        <v>2</v>
+      </c>
+      <c r="E21" s="15">
+        <v>8.7055056329612412E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="16">
+        <v>3</v>
+      </c>
+      <c r="E22" s="15">
+        <v>8.027415617602307E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="16">
         <v>4</v>
       </c>
-      <c r="F10" s="26">
-        <v>22</v>
-      </c>
-      <c r="G10" s="26">
-        <v>2.5</v>
-      </c>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="27">
+      <c r="E23" s="15">
+        <v>7.5785828325519916E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="16">
+        <v>5</v>
+      </c>
+      <c r="E24" s="15">
+        <v>7.2477966367769556E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="16">
+        <v>6</v>
+      </c>
+      <c r="E25" s="15">
+        <v>6.988271187715793E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="16">
+        <v>7</v>
+      </c>
+      <c r="E26" s="15">
+        <v>6.776109134004811E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="16">
+        <v>8</v>
+      </c>
+      <c r="E27" s="15">
+        <v>6.5975395538644718E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="16">
+        <v>9</v>
+      </c>
+      <c r="E28" s="15">
+        <v>6.4439401497725424E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="16">
+        <v>10</v>
+      </c>
+      <c r="E29" s="15">
+        <v>6.3095734448019331E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="33" spans="2:8" ht="130.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="26">
-        <v>6</v>
-      </c>
-      <c r="F14" s="26">
-        <v>32</v>
-      </c>
-      <c r="G14" s="26">
-        <v>2.5</v>
-      </c>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="21" t="s">
+      <c r="F34" s="10">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="27">
-        <v>4</v>
-      </c>
-      <c r="E18" s="26">
-        <v>8</v>
-      </c>
-      <c r="F18" s="26">
-        <v>50</v>
-      </c>
-      <c r="G18" s="26">
-        <v>2</v>
-      </c>
-      <c r="H18" s="25"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="8">
-        <v>5</v>
-      </c>
-      <c r="E22" s="23">
-        <v>10</v>
-      </c>
-      <c r="F22" s="22">
-        <v>75</v>
-      </c>
-      <c r="G22" s="22">
-        <v>2</v>
-      </c>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="G34" s="10">
         <v>30</v>
       </c>
-      <c r="D24" s="8">
-        <v>6</v>
-      </c>
-      <c r="E24" s="23">
-        <v>12</v>
-      </c>
-      <c r="F24" s="22">
-        <v>120</v>
-      </c>
-      <c r="G24" s="22">
-        <v>2</v>
-      </c>
-      <c r="H24" s="21"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="8">
-        <v>7</v>
-      </c>
-      <c r="E26" s="23">
-        <v>14</v>
-      </c>
-      <c r="F26" s="22">
-        <v>5000</v>
-      </c>
-      <c r="G26" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="8">
-        <v>8</v>
-      </c>
-      <c r="E28" s="23">
-        <v>16</v>
-      </c>
-      <c r="F28" s="22">
-        <v>5000</v>
-      </c>
-      <c r="G28" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="H28" s="21"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="35" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="17">
-        <v>1</v>
-      </c>
-      <c r="E36" s="16">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="17">
-        <v>2</v>
-      </c>
-      <c r="E37" s="16">
-        <v>8.7055056329612412E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="17">
-        <v>3</v>
-      </c>
-      <c r="E38" s="16">
-        <v>8.027415617602307E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="17">
-        <v>4</v>
-      </c>
-      <c r="E39" s="16">
-        <v>7.5785828325519916E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="17">
-        <v>5</v>
-      </c>
-      <c r="E40" s="16">
-        <v>7.2477966367769556E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="17">
-        <v>6</v>
-      </c>
-      <c r="E41" s="16">
-        <v>6.988271187715793E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="17">
-        <v>7</v>
-      </c>
-      <c r="E42" s="16">
-        <v>6.776109134004811E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="17">
-        <v>8</v>
-      </c>
-      <c r="E43" s="16">
-        <v>6.5975395538644718E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="17">
-        <v>9</v>
-      </c>
-      <c r="E44" s="16">
-        <v>6.4439401497725424E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="17">
-        <v>10</v>
-      </c>
-      <c r="E45" s="16">
-        <v>6.3095734448019331E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B47" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="49" spans="2:8" ht="130.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F50" s="11">
-        <v>50</v>
-      </c>
-      <c r="G50" s="11">
-        <v>30</v>
-      </c>
-      <c r="H50" s="11">
+      <c r="H34" s="10">
         <v>20</v>
       </c>
     </row>
@@ -1931,8 +1675,8 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="H5:H29"/>
-    <dataValidation allowBlank="1" sqref="E36:F45 E5:G29"/>
+    <dataValidation allowBlank="1" sqref="E20:F29 E5:G13" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="H5:H13" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>